<commit_message>
#21 feat alpine 버전 제거, 엑셀변경
</commit_message>
<xml_diff>
--- a/webterview_be/src/main/resources/example/면접관.xlsx
+++ b/webterview_be/src/main/resources/example/면접관.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abcd_\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9E0512-5BE0-4C71-8068-95A7F4B8F2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6419D69-1794-4A6B-A324-1F7ED8978F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -438,33 +438,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>